<commit_message>
properly indents time scales on left and right alignments...
</commit_message>
<xml_diff>
--- a/Private-Weekly-Productivity-Log.xlsx
+++ b/Private-Weekly-Productivity-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/867acb827b40e744/Desktop/PROJECTS/Sheetz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="14_{92C45805-CC96-491F-80CF-DA8B928F92F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E781B52-D2DC-41B8-8555-F005F92B4378}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="14_{92C45805-CC96-491F-80CF-DA8B928F92F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F71B8C18-ED0F-4FE4-B89C-71B3F183CE3E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -749,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
@@ -950,6 +950,33 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2272,6 +2299,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6521,14 +6552,15 @@
   </sheetPr>
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="76" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="88.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.85546875" customWidth="1"/>
@@ -6536,7 +6568,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60"/>
+      <c r="A1" s="68"/>
       <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
@@ -6558,7 +6590,7 @@
       <c r="H1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="60"/>
+      <c r="I1" s="70"/>
       <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
@@ -6573,7 +6605,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61"/>
+      <c r="A2" s="69"/>
       <c r="B2" s="51" t="s">
         <v>32</v>
       </c>
@@ -6595,7 +6627,7 @@
       <c r="H2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="61"/>
+      <c r="I2" s="71"/>
       <c r="J2" s="35" t="s">
         <v>13</v>
       </c>
@@ -6610,7 +6642,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47">
+      <c r="A3" s="72">
         <v>0</v>
       </c>
       <c r="B3" s="48"/>
@@ -6635,7 +6667,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37">
+      <c r="A4" s="73">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="B4" s="45"/>
@@ -6662,7 +6694,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
+      <c r="A5" s="74">
         <v>2.0833333333333301E-2</v>
       </c>
       <c r="B5" s="44"/>
@@ -6689,7 +6721,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
+      <c r="A6" s="73">
         <v>3.125E-2</v>
       </c>
       <c r="B6" s="45"/>
@@ -6716,7 +6748,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36">
+      <c r="A7" s="74">
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="B7" s="44"/>
@@ -6743,7 +6775,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
+      <c r="A8" s="73">
         <v>5.2083333333333301E-2</v>
       </c>
       <c r="B8" s="45"/>
@@ -6768,7 +6800,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36">
+      <c r="A9" s="74">
         <v>6.25E-2</v>
       </c>
       <c r="B9" s="44"/>
@@ -6795,7 +6827,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37">
+      <c r="A10" s="73">
         <v>7.2916666666666699E-2</v>
       </c>
       <c r="B10" s="45"/>
@@ -6822,7 +6854,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36">
+      <c r="A11" s="74">
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="B11" s="44"/>
@@ -6849,7 +6881,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37">
+      <c r="A12" s="73">
         <v>9.375E-2</v>
       </c>
       <c r="B12" s="45"/>
@@ -6876,7 +6908,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36">
+      <c r="A13" s="74">
         <v>0.104166666666667</v>
       </c>
       <c r="B13" s="44"/>
@@ -6891,7 +6923,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37">
+      <c r="A14" s="73">
         <v>0.114583333333333</v>
       </c>
       <c r="B14" s="45"/>
@@ -6906,7 +6938,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36">
+      <c r="A15" s="74">
         <v>0.125</v>
       </c>
       <c r="B15" s="44"/>
@@ -6921,7 +6953,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37">
+      <c r="A16" s="73">
         <v>0.13541666666666699</v>
       </c>
       <c r="B16" s="45"/>
@@ -6936,7 +6968,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36">
+      <c r="A17" s="74">
         <v>0.14583333333333301</v>
       </c>
       <c r="B17" s="44"/>
@@ -6951,7 +6983,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37">
+      <c r="A18" s="73">
         <v>0.15625</v>
       </c>
       <c r="B18" s="45"/>
@@ -6966,7 +6998,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36">
+      <c r="A19" s="74">
         <v>0.16666666666666699</v>
       </c>
       <c r="B19" s="44"/>
@@ -6981,7 +7013,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37">
+      <c r="A20" s="73">
         <v>0.17708333333333301</v>
       </c>
       <c r="B20" s="45"/>
@@ -6996,7 +7028,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36">
+      <c r="A21" s="74">
         <v>0.1875</v>
       </c>
       <c r="B21" s="44"/>
@@ -7011,7 +7043,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37">
+      <c r="A22" s="73">
         <v>0.19791666666666699</v>
       </c>
       <c r="B22" s="54"/>
@@ -7026,7 +7058,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="36">
+      <c r="A23" s="74">
         <v>0.20833333333333301</v>
       </c>
       <c r="B23" s="62" t="s">
@@ -7043,7 +7075,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37">
+      <c r="A24" s="73">
         <v>0.21875</v>
       </c>
       <c r="B24" s="57"/>
@@ -7062,7 +7094,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36">
+      <c r="A25" s="74">
         <v>0.22916666666666699</v>
       </c>
       <c r="B25" s="44"/>
@@ -7081,7 +7113,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37">
+      <c r="A26" s="73">
         <v>0.23958333333333301</v>
       </c>
       <c r="B26" s="45"/>
@@ -7100,7 +7132,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="36">
+      <c r="A27" s="74">
         <v>0.25</v>
       </c>
       <c r="B27" s="44"/>
@@ -7119,7 +7151,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37">
+      <c r="A28" s="73">
         <v>0.26041666666666702</v>
       </c>
       <c r="B28" s="45"/>
@@ -7138,7 +7170,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="36">
+      <c r="A29" s="74">
         <v>0.27083333333333298</v>
       </c>
       <c r="B29" s="44"/>
@@ -7157,7 +7189,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37">
+      <c r="A30" s="73">
         <v>0.28125</v>
       </c>
       <c r="B30" s="45"/>
@@ -7176,7 +7208,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="36">
+      <c r="A31" s="74">
         <v>0.29166666666666702</v>
       </c>
       <c r="B31" s="44"/>
@@ -7195,7 +7227,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37">
+      <c r="A32" s="73">
         <v>0.30208333333333298</v>
       </c>
       <c r="B32" s="45"/>
@@ -7214,7 +7246,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36">
+      <c r="A33" s="74">
         <v>0.3125</v>
       </c>
       <c r="B33" s="44"/>
@@ -7233,7 +7265,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37">
+      <c r="A34" s="73">
         <v>0.32291666666666702</v>
       </c>
       <c r="B34" s="45"/>
@@ -7252,7 +7284,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="36">
+      <c r="A35" s="74">
         <v>0.33333333333333298</v>
       </c>
       <c r="B35" s="44"/>
@@ -7271,7 +7303,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="37">
+      <c r="A36" s="73">
         <v>0.343749999999999</v>
       </c>
       <c r="B36" s="45"/>
@@ -7290,7 +7322,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="36">
+      <c r="A37" s="74">
         <v>0.35416666666666502</v>
       </c>
       <c r="B37" s="44"/>
@@ -7305,7 +7337,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37">
+      <c r="A38" s="73">
         <v>0.36458333333333098</v>
       </c>
       <c r="B38" s="45"/>
@@ -7320,7 +7352,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="36">
+      <c r="A39" s="74">
         <v>0.374999999999997</v>
       </c>
       <c r="B39" s="44"/>
@@ -7339,7 +7371,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37">
+      <c r="A40" s="73">
         <v>0.38541666666666302</v>
       </c>
       <c r="B40" s="45"/>
@@ -7358,7 +7390,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="36">
+      <c r="A41" s="74">
         <v>0.39583333333332898</v>
       </c>
       <c r="B41" s="44"/>
@@ -7377,7 +7409,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37">
+      <c r="A42" s="73">
         <v>0.406249999999995</v>
       </c>
       <c r="B42" s="45"/>
@@ -7396,7 +7428,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="36">
+      <c r="A43" s="74">
         <v>0.41666666666666102</v>
       </c>
       <c r="B43" s="44"/>
@@ -7411,7 +7443,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="37">
+      <c r="A44" s="73">
         <v>0.42708333333332699</v>
       </c>
       <c r="B44" s="45"/>
@@ -7426,7 +7458,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="36">
+      <c r="A45" s="74">
         <v>0.43749999999999301</v>
       </c>
       <c r="B45" s="44"/>
@@ -7443,7 +7475,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="37">
+      <c r="A46" s="73">
         <v>0.44791666666665902</v>
       </c>
       <c r="B46" s="45"/>
@@ -7460,7 +7492,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="36">
+      <c r="A47" s="74">
         <v>0.45833333333332499</v>
       </c>
       <c r="B47" s="44" t="s">
@@ -7477,7 +7509,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="37">
+      <c r="A48" s="73">
         <v>0.46874999999999101</v>
       </c>
       <c r="B48" s="45" t="s">
@@ -7494,7 +7526,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="36">
+      <c r="A49" s="74">
         <v>0.47916666666665703</v>
       </c>
       <c r="B49" s="45" t="s">
@@ -7513,7 +7545,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="37">
+      <c r="A50" s="73">
         <v>0.48958333333332299</v>
       </c>
       <c r="B50" s="45" t="s">
@@ -7532,7 +7564,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="36">
+      <c r="A51" s="74">
         <v>0.49999999999998901</v>
       </c>
       <c r="B51" s="44"/>
@@ -7551,7 +7583,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="37">
+      <c r="A52" s="73">
         <v>0.51041666666665497</v>
       </c>
       <c r="B52" s="45"/>
@@ -7570,7 +7602,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="36">
+      <c r="A53" s="74">
         <v>0.52083333333332105</v>
       </c>
       <c r="B53" s="44" t="s">
@@ -7591,7 +7623,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="37">
+      <c r="A54" s="73">
         <v>0.53124999999998701</v>
       </c>
       <c r="B54" s="44" t="s">
@@ -7612,7 +7644,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="36">
+      <c r="A55" s="74">
         <v>0.54166666666665297</v>
       </c>
       <c r="B55" s="44" t="s">
@@ -7633,7 +7665,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="37">
+      <c r="A56" s="73">
         <v>0.55208333333331905</v>
       </c>
       <c r="B56" s="44" t="s">
@@ -7652,7 +7684,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="36">
+      <c r="A57" s="74">
         <v>0.56249999999998501</v>
       </c>
       <c r="B57" s="44" t="s">
@@ -7671,7 +7703,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="37">
+      <c r="A58" s="73">
         <v>0.57291666666665098</v>
       </c>
       <c r="B58" s="44" t="s">
@@ -7690,7 +7722,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="36">
+      <c r="A59" s="74">
         <v>0.58333333333331705</v>
       </c>
       <c r="B59" s="44" t="s">
@@ -7707,7 +7739,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="37">
+      <c r="A60" s="73">
         <v>0.59374999999998201</v>
       </c>
       <c r="B60" s="44" t="s">
@@ -7724,7 +7756,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="36">
+      <c r="A61" s="74">
         <v>0.60416666666664798</v>
       </c>
       <c r="B61" s="44" t="s">
@@ -7741,7 +7773,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="37">
+      <c r="A62" s="73">
         <v>0.61458333333331405</v>
       </c>
       <c r="B62" s="44" t="s">
@@ -7758,7 +7790,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="36">
+      <c r="A63" s="74">
         <v>0.62499999999998002</v>
       </c>
       <c r="B63" s="44" t="s">
@@ -7777,7 +7809,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="37">
+      <c r="A64" s="73">
         <v>0.63541666666664598</v>
       </c>
       <c r="B64" s="44" t="s">
@@ -7796,7 +7828,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="36">
+      <c r="A65" s="74">
         <v>0.64583333333331205</v>
       </c>
       <c r="B65" s="44" t="s">
@@ -7815,7 +7847,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="37">
+      <c r="A66" s="73">
         <v>0.65624999999997802</v>
       </c>
       <c r="B66" s="44" t="s">
@@ -7834,7 +7866,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="36">
+      <c r="A67" s="74">
         <v>0.66666666666664398</v>
       </c>
       <c r="B67" s="44"/>
@@ -7851,7 +7883,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="37">
+      <c r="A68" s="73">
         <v>0.67708333333330994</v>
       </c>
       <c r="B68" s="44"/>
@@ -7868,7 +7900,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="36">
+      <c r="A69" s="74">
         <v>0.68749999999997602</v>
       </c>
       <c r="B69" s="44" t="s">
@@ -7887,7 +7919,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="37">
+      <c r="A70" s="73">
         <v>0.69791666666664198</v>
       </c>
       <c r="B70" s="44" t="s">
@@ -7906,7 +7938,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="36">
+      <c r="A71" s="74">
         <v>0.70833333333330795</v>
       </c>
       <c r="B71" s="44" t="s">
@@ -7923,7 +7955,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="37">
+      <c r="A72" s="73">
         <v>0.71874999999997402</v>
       </c>
       <c r="B72" s="44" t="s">
@@ -7940,7 +7972,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="36">
+      <c r="A73" s="74">
         <v>0.72916666666663998</v>
       </c>
       <c r="B73" s="44" t="s">
@@ -7957,7 +7989,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="37">
+      <c r="A74" s="73">
         <v>0.73958333333330595</v>
       </c>
       <c r="B74" s="44" t="s">
@@ -7974,7 +8006,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="36">
+      <c r="A75" s="74">
         <v>0.74999999999997202</v>
       </c>
       <c r="B75" s="44" t="s">
@@ -7993,7 +8025,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="37">
+      <c r="A76" s="73">
         <v>0.76041666666663799</v>
       </c>
       <c r="B76" s="44" t="s">
@@ -8012,7 +8044,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="36">
+      <c r="A77" s="74">
         <v>0.77083333333330395</v>
       </c>
       <c r="B77" s="44" t="s">
@@ -8031,7 +8063,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="37">
+      <c r="A78" s="73">
         <v>0.78124999999997002</v>
       </c>
       <c r="B78" s="45"/>
@@ -8048,7 +8080,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="36">
+      <c r="A79" s="74">
         <v>0.79166666666663699</v>
       </c>
       <c r="B79" s="44"/>
@@ -8065,7 +8097,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="37">
+      <c r="A80" s="73">
         <v>0.80208333333330295</v>
       </c>
       <c r="B80" s="45"/>
@@ -8082,7 +8114,7 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="36">
+      <c r="A81" s="74">
         <v>0.81249999999996902</v>
       </c>
       <c r="B81" s="44"/>
@@ -8099,7 +8131,7 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="37">
+      <c r="A82" s="73">
         <v>0.82291666666663499</v>
       </c>
       <c r="B82" s="45"/>
@@ -8116,7 +8148,7 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="36">
+      <c r="A83" s="74">
         <v>0.83333333333330095</v>
       </c>
       <c r="B83" s="44"/>
@@ -8133,7 +8165,7 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="37">
+      <c r="A84" s="73">
         <v>0.84374999999996703</v>
       </c>
       <c r="B84" s="45"/>
@@ -8150,7 +8182,7 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="36">
+      <c r="A85" s="74">
         <v>0.85416666666663299</v>
       </c>
       <c r="B85" s="44" t="s">
@@ -8169,7 +8201,7 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="37">
+      <c r="A86" s="73">
         <v>0.86458333333329895</v>
       </c>
       <c r="B86" s="54" t="s">
@@ -8188,7 +8220,7 @@
       </c>
     </row>
     <row r="87" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="36">
+      <c r="A87" s="74">
         <v>0.87499999999996303</v>
       </c>
       <c r="B87" s="62" t="s">
@@ -8205,7 +8237,7 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="37">
+      <c r="A88" s="73">
         <v>0.88541666666662899</v>
       </c>
       <c r="B88" s="57" t="s">
@@ -8222,7 +8254,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="36">
+      <c r="A89" s="74">
         <v>0.89583333333329496</v>
       </c>
       <c r="B89" s="44" t="s">
@@ -8239,7 +8271,7 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="37">
+      <c r="A90" s="73">
         <v>0.90624999999996103</v>
       </c>
       <c r="B90" s="45"/>
@@ -8254,7 +8286,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="36">
+      <c r="A91" s="74">
         <v>0.91666666666662699</v>
       </c>
       <c r="B91" s="44"/>
@@ -8269,7 +8301,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="37">
+      <c r="A92" s="73">
         <v>0.92708333333329296</v>
       </c>
       <c r="B92" s="45"/>
@@ -8284,7 +8316,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="36">
+      <c r="A93" s="74">
         <v>0.93749999999995903</v>
       </c>
       <c r="B93" s="44"/>
@@ -8299,7 +8331,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="37">
+      <c r="A94" s="73">
         <v>0.947916666666625</v>
       </c>
       <c r="B94" s="45"/>
@@ -8314,7 +8346,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="36">
+      <c r="A95" s="74">
         <v>0.95833333333329096</v>
       </c>
       <c r="B95" s="44"/>
@@ -8329,7 +8361,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="37">
+      <c r="A96" s="73">
         <v>0.96874999999995703</v>
       </c>
       <c r="B96" s="45"/>
@@ -8344,7 +8376,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="36">
+      <c r="A97" s="74">
         <v>0.979166666666623</v>
       </c>
       <c r="B97" s="44"/>
@@ -8359,7 +8391,7 @@
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="38">
+      <c r="A98" s="75">
         <v>0.98958333333328896</v>
       </c>
       <c r="B98" s="46"/>

</xml_diff>

<commit_message>
makes .gitignore fr this time
</commit_message>
<xml_diff>
--- a/Private-Weekly-Productivity-Log.xlsx
+++ b/Private-Weekly-Productivity-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/867acb827b40e744/Desktop/PROJECTS/Sheetz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="14_{92C45805-CC96-491F-80CF-DA8B928F92F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F71B8C18-ED0F-4FE4-B89C-71B3F183CE3E}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="14_{92C45805-CC96-491F-80CF-DA8B928F92F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D23517A8-8C18-408A-B263-E17934970E2A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="56">
   <si>
     <t>MON</t>
   </si>
@@ -926,6 +926,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="1" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -962,21 +977,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,21 +985,49 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFA2B6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB0E57C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD8BFD8"/>
+          <bgColor rgb="FF7AA5CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66CC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1014,98 +1042,42 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66CC77"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7AA5CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7AA5CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66CC77"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF999999"/>
+          <bgColor rgb="FFD8BFD8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB0E57C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA2B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA2B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB0E57C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD8BFD8"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1120,21 +1092,49 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFD8BFD8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB0E57C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFA2B6"/>
+          <bgColor rgb="FF999999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66CC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7AA5CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2299,10 +2299,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2653,7 +2649,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60"/>
+      <c r="A1" s="65"/>
       <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
@@ -2675,7 +2671,7 @@
       <c r="H1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="60"/>
+      <c r="I1" s="65"/>
       <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
@@ -2690,7 +2686,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61"/>
+      <c r="A2" s="66"/>
       <c r="B2" s="51" t="s">
         <v>32</v>
       </c>
@@ -2712,7 +2708,7 @@
       <c r="H2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="61"/>
+      <c r="I2" s="66"/>
       <c r="J2" s="35" t="s">
         <v>13</v>
       </c>
@@ -3147,15 +3143,15 @@
       <c r="A23" s="36">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="64"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="69"/>
       <c r="I23" s="36">
         <v>0.20833333333333301</v>
       </c>
@@ -4109,15 +4105,15 @@
       <c r="A87" s="36">
         <v>0.87499999999996303</v>
       </c>
-      <c r="B87" s="62" t="s">
+      <c r="B87" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C87" s="63"/>
-      <c r="D87" s="63"/>
-      <c r="E87" s="63"/>
-      <c r="F87" s="63"/>
-      <c r="G87" s="63"/>
-      <c r="H87" s="64"/>
+      <c r="C87" s="68"/>
+      <c r="D87" s="68"/>
+      <c r="E87" s="68"/>
+      <c r="F87" s="68"/>
+      <c r="G87" s="68"/>
+      <c r="H87" s="69"/>
       <c r="I87" s="36">
         <v>0.87499999999996303</v>
       </c>
@@ -4534,15 +4530,15 @@
       <c r="A13" s="31">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="67"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="72"/>
       <c r="J13" s="11" t="s">
         <v>9</v>
       </c>
@@ -5142,15 +5138,15 @@
       <c r="A45" s="31">
         <v>0.875</v>
       </c>
-      <c r="B45" s="65" t="s">
+      <c r="B45" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="66"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="66"/>
-      <c r="F45" s="66"/>
-      <c r="G45" s="66"/>
-      <c r="H45" s="67"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
+      <c r="G45" s="71"/>
+      <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
@@ -5337,7 +5333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB105AFA-97B6-4C07-833E-C9B2EF2AB6C1}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B45" sqref="B45:H45"/>
     </sheetView>
   </sheetViews>
@@ -5523,15 +5519,15 @@
       <c r="A13" s="31">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="67"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="72"/>
       <c r="J13" s="11" t="s">
         <v>9</v>
       </c>
@@ -6379,15 +6375,15 @@
       <c r="A45" s="31">
         <v>0.875</v>
       </c>
-      <c r="B45" s="65" t="s">
+      <c r="B45" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="66"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="66"/>
-      <c r="F45" s="66"/>
-      <c r="G45" s="66"/>
-      <c r="H45" s="67"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
+      <c r="G45" s="71"/>
+      <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
@@ -6552,13 +6548,13 @@
   </sheetPr>
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="76" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="64" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -6568,7 +6564,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68"/>
+      <c r="A1" s="73"/>
       <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
@@ -6590,7 +6586,7 @@
       <c r="H1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="70"/>
+      <c r="I1" s="75"/>
       <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
@@ -6605,29 +6601,29 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="71"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="51">
+        <v>45271</v>
+      </c>
+      <c r="C2" s="51">
+        <v>45272</v>
+      </c>
+      <c r="D2" s="51">
+        <v>45273</v>
+      </c>
+      <c r="E2" s="51">
+        <v>45274</v>
+      </c>
+      <c r="F2" s="51">
+        <v>45275</v>
+      </c>
+      <c r="G2" s="51">
+        <v>45276</v>
+      </c>
+      <c r="H2" s="51">
+        <v>45277</v>
+      </c>
+      <c r="I2" s="76"/>
       <c r="J2" s="35" t="s">
         <v>13</v>
       </c>
@@ -6642,7 +6638,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72">
+      <c r="A3" s="60">
         <v>0</v>
       </c>
       <c r="B3" s="48"/>
@@ -6667,7 +6663,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="73">
+      <c r="A4" s="61">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="B4" s="45"/>
@@ -6694,7 +6690,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74">
+      <c r="A5" s="62">
         <v>2.0833333333333301E-2</v>
       </c>
       <c r="B5" s="44"/>
@@ -6721,7 +6717,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="73">
+      <c r="A6" s="61">
         <v>3.125E-2</v>
       </c>
       <c r="B6" s="45"/>
@@ -6748,7 +6744,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="74">
+      <c r="A7" s="62">
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="B7" s="44"/>
@@ -6775,7 +6771,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73">
+      <c r="A8" s="61">
         <v>5.2083333333333301E-2</v>
       </c>
       <c r="B8" s="45"/>
@@ -6800,7 +6796,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="74">
+      <c r="A9" s="62">
         <v>6.25E-2</v>
       </c>
       <c r="B9" s="44"/>
@@ -6827,7 +6823,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73">
+      <c r="A10" s="61">
         <v>7.2916666666666699E-2</v>
       </c>
       <c r="B10" s="45"/>
@@ -6854,7 +6850,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="74">
+      <c r="A11" s="62">
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="B11" s="44"/>
@@ -6881,7 +6877,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="73">
+      <c r="A12" s="61">
         <v>9.375E-2</v>
       </c>
       <c r="B12" s="45"/>
@@ -6908,7 +6904,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="74">
+      <c r="A13" s="62">
         <v>0.104166666666667</v>
       </c>
       <c r="B13" s="44"/>
@@ -6923,7 +6919,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73">
+      <c r="A14" s="61">
         <v>0.114583333333333</v>
       </c>
       <c r="B14" s="45"/>
@@ -6938,7 +6934,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="74">
+      <c r="A15" s="62">
         <v>0.125</v>
       </c>
       <c r="B15" s="44"/>
@@ -6953,7 +6949,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73">
+      <c r="A16" s="61">
         <v>0.13541666666666699</v>
       </c>
       <c r="B16" s="45"/>
@@ -6968,7 +6964,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="74">
+      <c r="A17" s="62">
         <v>0.14583333333333301</v>
       </c>
       <c r="B17" s="44"/>
@@ -6983,7 +6979,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="73">
+      <c r="A18" s="61">
         <v>0.15625</v>
       </c>
       <c r="B18" s="45"/>
@@ -6998,7 +6994,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="74">
+      <c r="A19" s="62">
         <v>0.16666666666666699</v>
       </c>
       <c r="B19" s="44"/>
@@ -7013,7 +7009,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73">
+      <c r="A20" s="61">
         <v>0.17708333333333301</v>
       </c>
       <c r="B20" s="45"/>
@@ -7028,7 +7024,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="74">
+      <c r="A21" s="62">
         <v>0.1875</v>
       </c>
       <c r="B21" s="44"/>
@@ -7043,7 +7039,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="73">
+      <c r="A22" s="61">
         <v>0.19791666666666699</v>
       </c>
       <c r="B22" s="54"/>
@@ -7058,24 +7054,24 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="74">
+      <c r="A23" s="62">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="64"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="69"/>
       <c r="I23" s="36">
         <v>0.20833333333333301</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73">
+      <c r="A24" s="61">
         <v>0.21875</v>
       </c>
       <c r="B24" s="57"/>
@@ -7085,7 +7081,9 @@
       <c r="D24" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="58"/>
+      <c r="E24" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F24" s="58"/>
       <c r="G24" s="58"/>
       <c r="H24" s="59"/>
@@ -7094,7 +7092,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74">
+      <c r="A25" s="62">
         <v>0.22916666666666699</v>
       </c>
       <c r="B25" s="44"/>
@@ -7104,7 +7102,9 @@
       <c r="D25" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="29"/>
+      <c r="E25" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="33"/>
@@ -7113,7 +7113,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="73">
+      <c r="A26" s="61">
         <v>0.23958333333333301</v>
       </c>
       <c r="B26" s="45"/>
@@ -7123,7 +7123,9 @@
       <c r="D26" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="34"/>
@@ -7132,7 +7134,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="74">
+      <c r="A27" s="62">
         <v>0.25</v>
       </c>
       <c r="B27" s="44"/>
@@ -7142,7 +7144,9 @@
       <c r="D27" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="29"/>
+      <c r="E27" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
       <c r="H27" s="33"/>
@@ -7151,7 +7155,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="73">
+      <c r="A28" s="61">
         <v>0.26041666666666702</v>
       </c>
       <c r="B28" s="45"/>
@@ -7161,7 +7165,9 @@
       <c r="D28" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="34"/>
@@ -7170,7 +7176,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="74">
+      <c r="A29" s="62">
         <v>0.27083333333333298</v>
       </c>
       <c r="B29" s="44"/>
@@ -7180,7 +7186,9 @@
       <c r="D29" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="29"/>
+      <c r="E29" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
       <c r="H29" s="33"/>
@@ -7189,7 +7197,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="73">
+      <c r="A30" s="61">
         <v>0.28125</v>
       </c>
       <c r="B30" s="45"/>
@@ -7199,7 +7207,9 @@
       <c r="D30" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="34"/>
@@ -7208,7 +7218,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="74">
+      <c r="A31" s="62">
         <v>0.29166666666666702</v>
       </c>
       <c r="B31" s="44"/>
@@ -7218,7 +7228,9 @@
       <c r="D31" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="29"/>
+      <c r="E31" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
       <c r="H31" s="33"/>
@@ -7227,7 +7239,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="73">
+      <c r="A32" s="61">
         <v>0.30208333333333298</v>
       </c>
       <c r="B32" s="45"/>
@@ -7237,7 +7249,9 @@
       <c r="D32" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="8"/>
+      <c r="E32" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="34"/>
@@ -7246,7 +7260,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="74">
+      <c r="A33" s="62">
         <v>0.3125</v>
       </c>
       <c r="B33" s="44"/>
@@ -7256,7 +7270,9 @@
       <c r="D33" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="29"/>
+      <c r="E33" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="33"/>
@@ -7265,7 +7281,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="73">
+      <c r="A34" s="61">
         <v>0.32291666666666702</v>
       </c>
       <c r="B34" s="45"/>
@@ -7284,7 +7300,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="74">
+      <c r="A35" s="62">
         <v>0.33333333333333298</v>
       </c>
       <c r="B35" s="44"/>
@@ -7294,7 +7310,9 @@
       <c r="D35" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="29"/>
+      <c r="E35" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="F35" s="29"/>
       <c r="G35" s="29"/>
       <c r="H35" s="33"/>
@@ -7303,7 +7321,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="73">
+      <c r="A36" s="61">
         <v>0.343749999999999</v>
       </c>
       <c r="B36" s="45"/>
@@ -7313,7 +7331,9 @@
       <c r="D36" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="34"/>
@@ -7322,13 +7342,15 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="74">
+      <c r="A37" s="62">
         <v>0.35416666666666502</v>
       </c>
       <c r="B37" s="44"/>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
+      <c r="E37" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="F37" s="29"/>
       <c r="G37" s="29"/>
       <c r="H37" s="33"/>
@@ -7337,13 +7359,15 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="73">
+      <c r="A38" s="61">
         <v>0.36458333333333098</v>
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="E38" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="34"/>
@@ -7352,7 +7376,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="74">
+      <c r="A39" s="62">
         <v>0.374999999999997</v>
       </c>
       <c r="B39" s="44"/>
@@ -7362,7 +7386,9 @@
       <c r="D39" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="29"/>
+      <c r="E39" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
       <c r="H39" s="33"/>
@@ -7371,7 +7397,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="73">
+      <c r="A40" s="61">
         <v>0.38541666666666302</v>
       </c>
       <c r="B40" s="45"/>
@@ -7390,7 +7416,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="74">
+      <c r="A41" s="62">
         <v>0.39583333333332898</v>
       </c>
       <c r="B41" s="44"/>
@@ -7409,7 +7435,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="73">
+      <c r="A42" s="61">
         <v>0.406249999999995</v>
       </c>
       <c r="B42" s="45"/>
@@ -7428,7 +7454,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="74">
+      <c r="A43" s="62">
         <v>0.41666666666666102</v>
       </c>
       <c r="B43" s="44"/>
@@ -7443,7 +7469,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="73">
+      <c r="A44" s="61">
         <v>0.42708333333332699</v>
       </c>
       <c r="B44" s="45"/>
@@ -7458,7 +7484,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="74">
+      <c r="A45" s="62">
         <v>0.43749999999999301</v>
       </c>
       <c r="B45" s="44"/>
@@ -7475,7 +7501,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="73">
+      <c r="A46" s="61">
         <v>0.44791666666665902</v>
       </c>
       <c r="B46" s="45"/>
@@ -7492,7 +7518,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="74">
+      <c r="A47" s="62">
         <v>0.45833333333332499</v>
       </c>
       <c r="B47" s="44" t="s">
@@ -7509,7 +7535,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="73">
+      <c r="A48" s="61">
         <v>0.46874999999999101</v>
       </c>
       <c r="B48" s="45" t="s">
@@ -7526,7 +7552,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="74">
+      <c r="A49" s="62">
         <v>0.47916666666665703</v>
       </c>
       <c r="B49" s="45" t="s">
@@ -7536,7 +7562,9 @@
         <v>16</v>
       </c>
       <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
+      <c r="E49" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="F49" s="29"/>
       <c r="G49" s="29"/>
       <c r="H49" s="33"/>
@@ -7545,7 +7573,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="73">
+      <c r="A50" s="61">
         <v>0.48958333333332299</v>
       </c>
       <c r="B50" s="45" t="s">
@@ -7564,7 +7592,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="74">
+      <c r="A51" s="62">
         <v>0.49999999999998901</v>
       </c>
       <c r="B51" s="44"/>
@@ -7583,7 +7611,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="73">
+      <c r="A52" s="61">
         <v>0.51041666666665497</v>
       </c>
       <c r="B52" s="45"/>
@@ -7593,7 +7621,9 @@
       <c r="D52" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E52" s="8"/>
+      <c r="E52" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
       <c r="H52" s="34"/>
@@ -7602,7 +7632,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="74">
+      <c r="A53" s="62">
         <v>0.52083333333332105</v>
       </c>
       <c r="B53" s="44" t="s">
@@ -7614,7 +7644,9 @@
       <c r="D53" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="29"/>
+      <c r="E53" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F53" s="29"/>
       <c r="G53" s="29"/>
       <c r="H53" s="33"/>
@@ -7623,7 +7655,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="73">
+      <c r="A54" s="61">
         <v>0.53124999999998701</v>
       </c>
       <c r="B54" s="44" t="s">
@@ -7635,7 +7667,9 @@
       <c r="D54" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="E54" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
       <c r="H54" s="34"/>
@@ -7644,7 +7678,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="74">
+      <c r="A55" s="62">
         <v>0.54166666666665297</v>
       </c>
       <c r="B55" s="44" t="s">
@@ -7665,7 +7699,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="73">
+      <c r="A56" s="61">
         <v>0.55208333333331905</v>
       </c>
       <c r="B56" s="44" t="s">
@@ -7675,7 +7709,9 @@
         <v>17</v>
       </c>
       <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+      <c r="E56" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
       <c r="H56" s="34"/>
@@ -7684,7 +7720,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="74">
+      <c r="A57" s="62">
         <v>0.56249999999998501</v>
       </c>
       <c r="B57" s="44" t="s">
@@ -7694,7 +7730,9 @@
       <c r="D57" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="29"/>
+      <c r="E57" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F57" s="29"/>
       <c r="G57" s="29"/>
       <c r="H57" s="33"/>
@@ -7703,7 +7741,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="73">
+      <c r="A58" s="61">
         <v>0.57291666666665098</v>
       </c>
       <c r="B58" s="44" t="s">
@@ -7713,7 +7751,9 @@
       <c r="D58" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="8"/>
+      <c r="E58" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
       <c r="H58" s="34"/>
@@ -7722,7 +7762,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="74">
+      <c r="A59" s="62">
         <v>0.58333333333331705</v>
       </c>
       <c r="B59" s="44" t="s">
@@ -7739,14 +7779,16 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="73">
+      <c r="A60" s="61">
         <v>0.59374999999998201</v>
       </c>
       <c r="B60" s="44" t="s">
         <v>41</v>
       </c>
       <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
+      <c r="D60" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
@@ -7756,7 +7798,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="74">
+      <c r="A61" s="62">
         <v>0.60416666666664798</v>
       </c>
       <c r="B61" s="44" t="s">
@@ -7773,7 +7815,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="73">
+      <c r="A62" s="61">
         <v>0.61458333333331405</v>
       </c>
       <c r="B62" s="44" t="s">
@@ -7790,7 +7832,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="74">
+      <c r="A63" s="62">
         <v>0.62499999999998002</v>
       </c>
       <c r="B63" s="44" t="s">
@@ -7799,7 +7841,9 @@
       <c r="C63" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="29"/>
+      <c r="D63" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="E63" s="29"/>
       <c r="F63" s="29"/>
       <c r="G63" s="29"/>
@@ -7809,7 +7853,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="73">
+      <c r="A64" s="61">
         <v>0.63541666666664598</v>
       </c>
       <c r="B64" s="44" t="s">
@@ -7828,7 +7872,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="74">
+      <c r="A65" s="62">
         <v>0.64583333333331205</v>
       </c>
       <c r="B65" s="44" t="s">
@@ -7837,7 +7881,9 @@
       <c r="C65" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="29"/>
+      <c r="D65" s="29" t="s">
+        <v>41</v>
+      </c>
       <c r="E65" s="29"/>
       <c r="F65" s="29"/>
       <c r="G65" s="29"/>
@@ -7847,7 +7893,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="73">
+      <c r="A66" s="61">
         <v>0.65624999999997802</v>
       </c>
       <c r="B66" s="44" t="s">
@@ -7856,7 +7902,9 @@
       <c r="C66" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D66" s="8"/>
+      <c r="D66" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
@@ -7866,14 +7914,16 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="74">
+      <c r="A67" s="62">
         <v>0.66666666666664398</v>
       </c>
       <c r="B67" s="44"/>
       <c r="C67" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D67" s="29"/>
+      <c r="D67" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="E67" s="29"/>
       <c r="F67" s="29"/>
       <c r="G67" s="29"/>
@@ -7883,14 +7933,16 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="73">
+      <c r="A68" s="61">
         <v>0.67708333333330994</v>
       </c>
       <c r="B68" s="44"/>
       <c r="C68" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D68" s="8"/>
+      <c r="D68" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
@@ -7900,7 +7952,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="74">
+      <c r="A69" s="62">
         <v>0.68749999999997602</v>
       </c>
       <c r="B69" s="44" t="s">
@@ -7909,7 +7961,9 @@
       <c r="C69" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D69" s="29"/>
+      <c r="D69" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="E69" s="29"/>
       <c r="F69" s="29"/>
       <c r="G69" s="29"/>
@@ -7919,7 +7973,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="73">
+      <c r="A70" s="61">
         <v>0.69791666666664198</v>
       </c>
       <c r="B70" s="44" t="s">
@@ -7928,7 +7982,9 @@
       <c r="C70" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D70" s="8"/>
+      <c r="D70" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
@@ -7938,14 +7994,16 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="74">
+      <c r="A71" s="62">
         <v>0.70833333333330795</v>
       </c>
       <c r="B71" s="44" t="s">
         <v>41</v>
       </c>
       <c r="C71" s="29"/>
-      <c r="D71" s="29"/>
+      <c r="D71" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="E71" s="29"/>
       <c r="F71" s="29"/>
       <c r="G71" s="29"/>
@@ -7955,14 +8013,16 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="73">
+      <c r="A72" s="61">
         <v>0.71874999999997402</v>
       </c>
       <c r="B72" s="44" t="s">
         <v>41</v>
       </c>
       <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
+      <c r="D72" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
@@ -7972,14 +8032,16 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="74">
+      <c r="A73" s="62">
         <v>0.72916666666663998</v>
       </c>
       <c r="B73" s="44" t="s">
         <v>41</v>
       </c>
       <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
+      <c r="D73" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="E73" s="29"/>
       <c r="F73" s="29"/>
       <c r="G73" s="29"/>
@@ -7989,7 +8051,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="73">
+      <c r="A74" s="61">
         <v>0.73958333333330595</v>
       </c>
       <c r="B74" s="44" t="s">
@@ -8006,7 +8068,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="74">
+      <c r="A75" s="62">
         <v>0.74999999999997202</v>
       </c>
       <c r="B75" s="44" t="s">
@@ -8025,7 +8087,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="73">
+      <c r="A76" s="61">
         <v>0.76041666666663799</v>
       </c>
       <c r="B76" s="44" t="s">
@@ -8044,7 +8106,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="74">
+      <c r="A77" s="62">
         <v>0.77083333333330395</v>
       </c>
       <c r="B77" s="44" t="s">
@@ -8053,7 +8115,9 @@
       <c r="C77" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D77" s="29"/>
+      <c r="D77" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="E77" s="29"/>
       <c r="F77" s="29"/>
       <c r="G77" s="29"/>
@@ -8063,14 +8127,16 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="73">
+      <c r="A78" s="61">
         <v>0.78124999999997002</v>
       </c>
       <c r="B78" s="45"/>
       <c r="C78" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="8"/>
+      <c r="D78" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
@@ -8080,14 +8146,16 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="74">
+      <c r="A79" s="62">
         <v>0.79166666666663699</v>
       </c>
       <c r="B79" s="44"/>
       <c r="C79" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D79" s="29"/>
+      <c r="D79" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="E79" s="29"/>
       <c r="F79" s="29"/>
       <c r="G79" s="29"/>
@@ -8097,14 +8165,16 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="73">
+      <c r="A80" s="61">
         <v>0.80208333333330295</v>
       </c>
       <c r="B80" s="45"/>
       <c r="C80" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D80" s="8"/>
+      <c r="D80" s="29" t="s">
+        <v>17</v>
+      </c>
       <c r="E80" s="8"/>
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
@@ -8114,14 +8184,16 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="74">
+      <c r="A81" s="62">
         <v>0.81249999999996902</v>
       </c>
       <c r="B81" s="44"/>
       <c r="C81" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D81" s="29"/>
+      <c r="D81" s="29" t="s">
+        <v>41</v>
+      </c>
       <c r="E81" s="29"/>
       <c r="F81" s="29"/>
       <c r="G81" s="29"/>
@@ -8131,14 +8203,16 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="73">
+      <c r="A82" s="61">
         <v>0.82291666666663499</v>
       </c>
       <c r="B82" s="45"/>
       <c r="C82" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D82" s="8"/>
+      <c r="D82" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="E82" s="8"/>
       <c r="F82" s="8"/>
       <c r="G82" s="8"/>
@@ -8148,14 +8222,16 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="74">
+      <c r="A83" s="62">
         <v>0.83333333333330095</v>
       </c>
       <c r="B83" s="44"/>
       <c r="C83" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D83" s="29"/>
+      <c r="D83" s="29" t="s">
+        <v>18</v>
+      </c>
       <c r="E83" s="29"/>
       <c r="F83" s="29"/>
       <c r="G83" s="29"/>
@@ -8165,7 +8241,7 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="73">
+      <c r="A84" s="61">
         <v>0.84374999999996703</v>
       </c>
       <c r="B84" s="45"/>
@@ -8182,7 +8258,7 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="74">
+      <c r="A85" s="62">
         <v>0.85416666666663299</v>
       </c>
       <c r="B85" s="44" t="s">
@@ -8201,7 +8277,7 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="73">
+      <c r="A86" s="61">
         <v>0.86458333333329895</v>
       </c>
       <c r="B86" s="54" t="s">
@@ -8220,24 +8296,24 @@
       </c>
     </row>
     <row r="87" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="74">
+      <c r="A87" s="62">
         <v>0.87499999999996303</v>
       </c>
-      <c r="B87" s="62" t="s">
+      <c r="B87" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C87" s="63"/>
-      <c r="D87" s="63"/>
-      <c r="E87" s="63"/>
-      <c r="F87" s="63"/>
-      <c r="G87" s="63"/>
-      <c r="H87" s="64"/>
+      <c r="C87" s="68"/>
+      <c r="D87" s="68"/>
+      <c r="E87" s="68"/>
+      <c r="F87" s="68"/>
+      <c r="G87" s="68"/>
+      <c r="H87" s="69"/>
       <c r="I87" s="36">
         <v>0.87499999999996303</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="73">
+      <c r="A88" s="61">
         <v>0.88541666666662899</v>
       </c>
       <c r="B88" s="57" t="s">
@@ -8254,7 +8330,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="74">
+      <c r="A89" s="62">
         <v>0.89583333333329496</v>
       </c>
       <c r="B89" s="44" t="s">
@@ -8271,7 +8347,7 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="73">
+      <c r="A90" s="61">
         <v>0.90624999999996103</v>
       </c>
       <c r="B90" s="45"/>
@@ -8286,7 +8362,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="74">
+      <c r="A91" s="62">
         <v>0.91666666666662699</v>
       </c>
       <c r="B91" s="44"/>
@@ -8301,7 +8377,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="73">
+      <c r="A92" s="61">
         <v>0.92708333333329296</v>
       </c>
       <c r="B92" s="45"/>
@@ -8316,7 +8392,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="74">
+      <c r="A93" s="62">
         <v>0.93749999999995903</v>
       </c>
       <c r="B93" s="44"/>
@@ -8331,7 +8407,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="73">
+      <c r="A94" s="61">
         <v>0.947916666666625</v>
       </c>
       <c r="B94" s="45"/>
@@ -8346,7 +8422,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="74">
+      <c r="A95" s="62">
         <v>0.95833333333329096</v>
       </c>
       <c r="B95" s="44"/>
@@ -8361,7 +8437,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="73">
+      <c r="A96" s="61">
         <v>0.96874999999995703</v>
       </c>
       <c r="B96" s="45"/>
@@ -8376,7 +8452,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="74">
+      <c r="A97" s="62">
         <v>0.979166666666623</v>
       </c>
       <c r="B97" s="44"/>
@@ -8391,7 +8467,7 @@
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="75">
+      <c r="A98" s="63">
         <v>0.98958333333328896</v>
       </c>
       <c r="B98" s="46"/>
@@ -8448,72 +8524,72 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:H86">
-    <cfRule type="expression" dxfId="21" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>B24=$J$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="13">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>B24=$J$11</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="14">
+    <cfRule type="expression" dxfId="8" priority="14">
       <formula>B24=$J$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="15">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>B24=$J$9</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="6" priority="16">
       <formula>B24=$J$8</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="5" priority="17">
       <formula>B24=$J$7</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="4" priority="18">
       <formula>B24=$J$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="19">
+    <cfRule type="expression" dxfId="3" priority="19">
       <formula>B24=$J$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="20">
+    <cfRule type="expression" dxfId="2" priority="20">
       <formula>B24=$J$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="21">
+    <cfRule type="expression" dxfId="1" priority="21">
       <formula>B24=$J$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="22">
+    <cfRule type="expression" dxfId="0" priority="22">
       <formula>B24=$J$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:H98">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="21" priority="11">
       <formula>B88=$J$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="20" priority="10">
       <formula>B88=$J$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="19" priority="9">
       <formula>B88=$J$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="18" priority="8">
       <formula>B88=$J$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>B88=$J$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>B88=$J$7</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>B88=$J$8</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>B88=$J$9</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>B88=$J$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>B88=$J$11</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>B88=$J$12</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>